<commit_message>
Correção de detecção de delimitador e outros ajustes
</commit_message>
<xml_diff>
--- a/data/fontes/Dimencoes.xlsx
+++ b/data/fontes/Dimencoes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abeil\Desktop\Mestrado\Qualidade dados\Planilhas de apoio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abeil\Documents\GitHub\DataQ-culture\data\fontes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34747698-4E3F-42E6-898D-540DCAC8BE71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5FF20E-C4AE-42A9-ADFA-59ADD6B4F576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B4AB4E59-3BB9-426B-9CE8-8252F7EB638E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B4AB4E59-3BB9-426B-9CE8-8252F7EB638E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -266,16 +258,16 @@
     <t>Measurements_Largura</t>
   </si>
   <si>
-    <t>Measurements_profundidade</t>
-  </si>
-  <si>
-    <t>Measurements_espessura</t>
-  </si>
-  <si>
-    <t>Measurements_diametro</t>
-  </si>
-  <si>
-    <t>Measurements_peso</t>
+    <t>Measurements_Profundidade</t>
+  </si>
+  <si>
+    <t>Measurements_Espessura</t>
+  </si>
+  <si>
+    <t>Measurements_Diametro</t>
+  </si>
+  <si>
+    <t>Measurements_Peso</t>
   </si>
 </sst>
 </file>
@@ -327,12 +319,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -342,7 +333,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -665,16 +656,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -682,7 +672,7 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -690,7 +680,7 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -698,7 +688,7 @@
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -706,7 +696,7 @@
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -714,7 +704,7 @@
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -722,7 +712,7 @@
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -730,7 +720,7 @@
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -738,7 +728,7 @@
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -746,7 +736,7 @@
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -754,7 +744,7 @@
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -762,7 +752,7 @@
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>25</v>
       </c>
     </row>
@@ -770,7 +760,7 @@
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
     </row>
@@ -778,7 +768,7 @@
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>27</v>
       </c>
     </row>
@@ -786,7 +776,7 @@
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -794,7 +784,7 @@
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -802,7 +792,7 @@
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -810,7 +800,7 @@
       <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>29</v>
       </c>
     </row>
@@ -818,7 +808,7 @@
       <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>30</v>
       </c>
     </row>
@@ -826,7 +816,7 @@
       <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -834,7 +824,7 @@
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -842,7 +832,7 @@
       <c r="A22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>32</v>
       </c>
     </row>
@@ -850,7 +840,7 @@
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>33</v>
       </c>
     </row>
@@ -858,7 +848,7 @@
       <c r="A24" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>34</v>
       </c>
     </row>
@@ -866,7 +856,7 @@
       <c r="A25" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -874,7 +864,7 @@
       <c r="A26" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -882,7 +872,7 @@
       <c r="A27" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -890,7 +880,7 @@
       <c r="A28" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>36</v>
       </c>
     </row>
@@ -898,7 +888,7 @@
       <c r="A29" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="2" t="s">
         <v>37</v>
       </c>
     </row>
@@ -906,7 +896,7 @@
       <c r="A30" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="3" t="s">
         <v>38</v>
       </c>
     </row>
@@ -914,7 +904,7 @@
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="3" t="s">
         <v>39</v>
       </c>
     </row>
@@ -922,7 +912,7 @@
       <c r="A32" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="3" t="s">
         <v>40</v>
       </c>
     </row>
@@ -930,7 +920,7 @@
       <c r="A33" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="2" t="s">
         <v>41</v>
       </c>
     </row>
@@ -938,7 +928,7 @@
       <c r="A34" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="3" t="s">
         <v>42</v>
       </c>
     </row>
@@ -946,7 +936,7 @@
       <c r="A35" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="3" t="s">
         <v>43</v>
       </c>
     </row>
@@ -954,7 +944,7 @@
       <c r="A36" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -962,7 +952,7 @@
       <c r="A37" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -970,7 +960,7 @@
       <c r="A38" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="2" t="s">
         <v>46</v>
       </c>
     </row>
@@ -978,7 +968,7 @@
       <c r="A39" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="3" t="s">
         <v>47</v>
       </c>
     </row>
@@ -986,7 +976,7 @@
       <c r="A40" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="3" t="s">
         <v>48</v>
       </c>
     </row>
@@ -994,7 +984,7 @@
       <c r="A41" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="3" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1002,7 +992,7 @@
       <c r="A42" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="3" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1010,7 +1000,7 @@
       <c r="A43" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="2" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1018,7 +1008,7 @@
       <c r="A44" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="2" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1026,7 +1016,7 @@
       <c r="A45" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="2" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1034,7 +1024,7 @@
       <c r="A46" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="2" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1042,7 +1032,7 @@
       <c r="A47" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="2" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1050,7 +1040,7 @@
       <c r="A48" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1058,7 +1048,7 @@
       <c r="A49" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="3" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1066,7 +1056,7 @@
       <c r="A50" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1074,7 +1064,7 @@
       <c r="A51" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="3" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1082,7 +1072,7 @@
       <c r="A52" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="3" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1090,7 +1080,7 @@
       <c r="A53" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="3" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1098,7 +1088,7 @@
       <c r="A54" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="3" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1106,7 +1096,7 @@
       <c r="A55" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1114,7 +1104,7 @@
       <c r="A56" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="3" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1122,7 +1112,7 @@
       <c r="A57" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="3" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1130,7 +1120,7 @@
       <c r="A58" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="2" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1138,7 +1128,7 @@
       <c r="A59" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="3" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1146,7 +1136,7 @@
       <c r="A60" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1154,7 +1144,7 @@
       <c r="A61" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="3" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1162,7 +1152,7 @@
       <c r="A62" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B62" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1170,7 +1160,7 @@
       <c r="A63" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1178,7 +1168,7 @@
       <c r="A64" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="3" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1186,7 +1176,7 @@
       <c r="A65" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1194,7 +1184,7 @@
       <c r="A66" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="3" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1202,7 +1192,7 @@
       <c r="A67" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B67" s="3" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1210,7 +1200,7 @@
       <c r="A68" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B68" s="3" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1218,7 +1208,7 @@
       <c r="A69" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B69" s="3" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1226,7 +1216,7 @@
       <c r="A70" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B70" s="3" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1234,55 +1224,55 @@
       <c r="A71" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B71" s="3" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B72" s="6" t="s">
+      <c r="A72" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B72" s="5" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B73" s="6" t="s">
+      <c r="A73" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B73" s="5" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B74" s="6" t="s">
+      <c r="A74" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B74" s="5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B75" s="6" t="s">
+      <c r="A75" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B75" s="5" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B76" s="6" t="s">
+      <c r="A76" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B76" s="5" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B77" s="6" t="s">
+      <c r="A77" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B77" s="5" t="s">
         <v>80</v>
       </c>
     </row>

</xml_diff>